<commit_message>
Programs done so far added
</commit_message>
<xml_diff>
--- a/Practice_Problems_for_Respective_Dates.xlsx
+++ b/Practice_Problems_for_Respective_Dates.xlsx
@@ -544,8 +544,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A6:E34"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B6" workbookViewId="0">
-      <selection activeCell="C20" sqref="C20"/>
+    <sheetView tabSelected="1" topLeftCell="C6" workbookViewId="0">
+      <selection activeCell="D20" sqref="D20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>

<commit_message>
Problem for Dec 21, 2020 added
</commit_message>
<xml_diff>
--- a/Practice_Problems_for_Respective_Dates.xlsx
+++ b/Practice_Problems_for_Respective_Dates.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="61" uniqueCount="56">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="65" uniqueCount="60">
   <si>
     <t>Date</t>
   </si>
@@ -192,6 +192,18 @@
   </si>
   <si>
     <t>Greater On Right Side</t>
+  </si>
+  <si>
+    <t>Dec 14, 2020</t>
+  </si>
+  <si>
+    <t>Majority Element</t>
+  </si>
+  <si>
+    <t>poDDec1420</t>
+  </si>
+  <si>
+    <t>Minimum and Maximum Element</t>
   </si>
 </sst>
 </file>
@@ -251,16 +263,25 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1"/>
-    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -542,10 +563,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A6:E34"/>
+  <dimension ref="A6:E35"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C6" workbookViewId="0">
-      <selection activeCell="D20" sqref="D20"/>
+    <sheetView tabSelected="1" topLeftCell="A6" workbookViewId="0">
+      <selection activeCell="C22" sqref="C22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -570,202 +591,215 @@
       <c r="E6" s="1"/>
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="B7" s="5" t="s">
+      <c r="B7" s="4" t="s">
         <v>3</v>
       </c>
-      <c r="C7" s="4" t="s">
+      <c r="C7" s="5" t="s">
         <v>4</v>
       </c>
-      <c r="D7" t="s">
+      <c r="D7" s="6" t="s">
         <v>14</v>
       </c>
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="B8" s="5" t="s">
+      <c r="B8" s="4" t="s">
         <v>5</v>
       </c>
-      <c r="C8" s="4" t="s">
+      <c r="C8" s="5" t="s">
         <v>6</v>
       </c>
-      <c r="D8" t="s">
+      <c r="D8" s="6" t="s">
         <v>15</v>
       </c>
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="B9" s="5" t="s">
+      <c r="B9" s="4" t="s">
         <v>8</v>
       </c>
-      <c r="C9" s="4" t="s">
+      <c r="C9" s="5" t="s">
         <v>7</v>
       </c>
-      <c r="D9" t="s">
+      <c r="D9" s="6" t="s">
         <v>16</v>
       </c>
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="B10" s="6" t="s">
+      <c r="B10" s="7" t="s">
         <v>10</v>
       </c>
-      <c r="C10" s="4" t="s">
+      <c r="C10" s="5" t="s">
         <v>9</v>
       </c>
-      <c r="D10" t="s">
+      <c r="D10" s="6" t="s">
         <v>17</v>
       </c>
     </row>
     <row r="11" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="B11" s="5" t="s">
+      <c r="B11" s="4" t="s">
         <v>12</v>
       </c>
-      <c r="C11" s="4" t="s">
+      <c r="C11" s="5" t="s">
         <v>11</v>
       </c>
-      <c r="D11" t="s">
+      <c r="D11" s="6" t="s">
         <v>18</v>
       </c>
     </row>
     <row r="12" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="B12" s="5" t="s">
+      <c r="B12" s="4" t="s">
         <v>19</v>
       </c>
-      <c r="C12" s="4" t="s">
+      <c r="C12" s="5" t="s">
         <v>20</v>
       </c>
-      <c r="D12" t="s">
+      <c r="D12" s="6" t="s">
         <v>21</v>
       </c>
     </row>
     <row r="13" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="B13" s="5" t="s">
+      <c r="B13" s="4" t="s">
         <v>23</v>
       </c>
-      <c r="C13" s="4" t="s">
+      <c r="C13" s="5" t="s">
         <v>22</v>
       </c>
-      <c r="D13" t="s">
+      <c r="D13" s="6" t="s">
         <v>24</v>
       </c>
     </row>
     <row r="14" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="B14" s="5" t="s">
+      <c r="B14" s="4" t="s">
         <v>26</v>
       </c>
-      <c r="C14" s="4" t="s">
+      <c r="C14" s="5" t="s">
         <v>25</v>
       </c>
-      <c r="D14" t="s">
+      <c r="D14" s="6" t="s">
         <v>35</v>
       </c>
     </row>
     <row r="15" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="B15" s="5" t="s">
+      <c r="B15" s="4" t="s">
         <v>27</v>
       </c>
-      <c r="C15" s="4" t="s">
+      <c r="C15" s="5" t="s">
         <v>29</v>
       </c>
-      <c r="D15" t="s">
+      <c r="D15" s="6" t="s">
         <v>36</v>
       </c>
     </row>
     <row r="16" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="B16" s="5" t="s">
+      <c r="B16" s="4" t="s">
         <v>30</v>
       </c>
-      <c r="C16" s="4" t="s">
+      <c r="C16" s="5" t="s">
         <v>28</v>
       </c>
-      <c r="D16" t="s">
+      <c r="D16" s="6" t="s">
         <v>37</v>
       </c>
     </row>
     <row r="17" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B17" s="5" t="s">
+      <c r="B17" s="4" t="s">
+        <v>56</v>
+      </c>
+      <c r="C17" s="5" t="s">
+        <v>57</v>
+      </c>
+      <c r="D17" s="6" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="18" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B18" s="4" t="s">
         <v>31</v>
       </c>
-      <c r="C17" s="4" t="s">
+      <c r="C18" s="5" t="s">
         <v>32</v>
       </c>
-      <c r="D17" t="s">
+      <c r="D18" s="6" t="s">
         <v>38</v>
       </c>
     </row>
-    <row r="18" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B18" s="5" t="s">
+    <row r="19" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B19" s="4" t="s">
         <v>34</v>
       </c>
-      <c r="C18" s="4" t="s">
+      <c r="C19" s="5" t="s">
         <v>33</v>
       </c>
-      <c r="D18" t="s">
+      <c r="D19" s="6" t="s">
         <v>39</v>
       </c>
     </row>
-    <row r="19" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B19" s="5" t="s">
+    <row r="20" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B20" s="4" t="s">
         <v>40</v>
       </c>
-      <c r="C19" s="4" t="s">
+      <c r="C20" s="5" t="s">
         <v>41</v>
       </c>
-      <c r="D19" t="s">
+      <c r="D20" s="6" t="s">
         <v>42</v>
       </c>
     </row>
-    <row r="20" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B20" s="5" t="s">
+    <row r="21" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B21" s="4" t="s">
         <v>43</v>
       </c>
-      <c r="C20" s="4" t="s">
+      <c r="C21" s="5" t="s">
         <v>55</v>
       </c>
-      <c r="D20" t="s">
+      <c r="D21" s="6" t="s">
         <v>49</v>
       </c>
     </row>
-    <row r="21" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B21" s="5" t="s">
+    <row r="22" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B22" s="4" t="s">
         <v>44</v>
       </c>
-      <c r="D21" t="s">
+      <c r="C22" s="5" t="s">
+        <v>59</v>
+      </c>
+      <c r="D22" s="6" t="s">
         <v>50</v>
       </c>
     </row>
-    <row r="22" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B22" s="5" t="s">
+    <row r="23" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B23" s="4" t="s">
         <v>45</v>
       </c>
-      <c r="D22" t="s">
+      <c r="C23" s="6"/>
+      <c r="D23" s="6" t="s">
         <v>51</v>
       </c>
     </row>
-    <row r="23" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B23" s="5" t="s">
+    <row r="24" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B24" s="4" t="s">
         <v>46</v>
       </c>
-      <c r="D23" t="s">
+      <c r="C24" s="6"/>
+      <c r="D24" s="6" t="s">
         <v>52</v>
       </c>
     </row>
-    <row r="24" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B24" s="5" t="s">
+    <row r="25" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B25" s="4" t="s">
         <v>47</v>
       </c>
-      <c r="D24" t="s">
+      <c r="C25" s="6"/>
+      <c r="D25" s="6" t="s">
         <v>53</v>
       </c>
     </row>
-    <row r="25" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B25" s="5" t="s">
+    <row r="26" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B26" s="4" t="s">
         <v>48</v>
       </c>
-      <c r="D25" t="s">
+      <c r="C26" s="6"/>
+      <c r="D26" s="6" t="s">
         <v>54</v>
-      </c>
-    </row>
-    <row r="29" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="D29" t="s">
-        <v>13</v>
       </c>
     </row>
     <row r="30" spans="2:4" x14ac:dyDescent="0.25">
@@ -790,6 +824,11 @@
     </row>
     <row r="34" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D34" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="35" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D35" t="s">
         <v>13</v>
       </c>
     </row>
@@ -805,11 +844,14 @@
     <hyperlink ref="C14" r:id="rId8"/>
     <hyperlink ref="C15" r:id="rId9"/>
     <hyperlink ref="C16" r:id="rId10"/>
-    <hyperlink ref="C17" r:id="rId11"/>
-    <hyperlink ref="C18" r:id="rId12"/>
-    <hyperlink ref="C19" r:id="rId13"/>
-    <hyperlink ref="C20" r:id="rId14"/>
+    <hyperlink ref="C18" r:id="rId11"/>
+    <hyperlink ref="C19" r:id="rId12"/>
+    <hyperlink ref="C20" r:id="rId13"/>
+    <hyperlink ref="C21" r:id="rId14"/>
+    <hyperlink ref="C17" r:id="rId15"/>
+    <hyperlink ref="C22" r:id="rId16"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId17"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Problem for Dec 20, 2020 added
</commit_message>
<xml_diff>
--- a/Practice_Problems_for_Respective_Dates.xlsx
+++ b/Practice_Problems_for_Respective_Dates.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="61" uniqueCount="56">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="65" uniqueCount="60">
   <si>
     <t>Date</t>
   </si>
@@ -192,6 +192,18 @@
   </si>
   <si>
     <t>Greater On Right Side</t>
+  </si>
+  <si>
+    <t>Dec 14, 2020</t>
+  </si>
+  <si>
+    <t>Majority Element</t>
+  </si>
+  <si>
+    <t>poDDec1420</t>
+  </si>
+  <si>
+    <t>Minimum and Maximum Element</t>
   </si>
 </sst>
 </file>
@@ -251,16 +263,25 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1"/>
-    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -542,10 +563,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A6:E34"/>
+  <dimension ref="A6:E35"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C6" workbookViewId="0">
-      <selection activeCell="D20" sqref="D20"/>
+    <sheetView tabSelected="1" topLeftCell="A6" workbookViewId="0">
+      <selection activeCell="C22" sqref="C22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -570,202 +591,215 @@
       <c r="E6" s="1"/>
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="B7" s="5" t="s">
+      <c r="B7" s="4" t="s">
         <v>3</v>
       </c>
-      <c r="C7" s="4" t="s">
+      <c r="C7" s="5" t="s">
         <v>4</v>
       </c>
-      <c r="D7" t="s">
+      <c r="D7" s="6" t="s">
         <v>14</v>
       </c>
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="B8" s="5" t="s">
+      <c r="B8" s="4" t="s">
         <v>5</v>
       </c>
-      <c r="C8" s="4" t="s">
+      <c r="C8" s="5" t="s">
         <v>6</v>
       </c>
-      <c r="D8" t="s">
+      <c r="D8" s="6" t="s">
         <v>15</v>
       </c>
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="B9" s="5" t="s">
+      <c r="B9" s="4" t="s">
         <v>8</v>
       </c>
-      <c r="C9" s="4" t="s">
+      <c r="C9" s="5" t="s">
         <v>7</v>
       </c>
-      <c r="D9" t="s">
+      <c r="D9" s="6" t="s">
         <v>16</v>
       </c>
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="B10" s="6" t="s">
+      <c r="B10" s="7" t="s">
         <v>10</v>
       </c>
-      <c r="C10" s="4" t="s">
+      <c r="C10" s="5" t="s">
         <v>9</v>
       </c>
-      <c r="D10" t="s">
+      <c r="D10" s="6" t="s">
         <v>17</v>
       </c>
     </row>
     <row r="11" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="B11" s="5" t="s">
+      <c r="B11" s="4" t="s">
         <v>12</v>
       </c>
-      <c r="C11" s="4" t="s">
+      <c r="C11" s="5" t="s">
         <v>11</v>
       </c>
-      <c r="D11" t="s">
+      <c r="D11" s="6" t="s">
         <v>18</v>
       </c>
     </row>
     <row r="12" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="B12" s="5" t="s">
+      <c r="B12" s="4" t="s">
         <v>19</v>
       </c>
-      <c r="C12" s="4" t="s">
+      <c r="C12" s="5" t="s">
         <v>20</v>
       </c>
-      <c r="D12" t="s">
+      <c r="D12" s="6" t="s">
         <v>21</v>
       </c>
     </row>
     <row r="13" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="B13" s="5" t="s">
+      <c r="B13" s="4" t="s">
         <v>23</v>
       </c>
-      <c r="C13" s="4" t="s">
+      <c r="C13" s="5" t="s">
         <v>22</v>
       </c>
-      <c r="D13" t="s">
+      <c r="D13" s="6" t="s">
         <v>24</v>
       </c>
     </row>
     <row r="14" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="B14" s="5" t="s">
+      <c r="B14" s="4" t="s">
         <v>26</v>
       </c>
-      <c r="C14" s="4" t="s">
+      <c r="C14" s="5" t="s">
         <v>25</v>
       </c>
-      <c r="D14" t="s">
+      <c r="D14" s="6" t="s">
         <v>35</v>
       </c>
     </row>
     <row r="15" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="B15" s="5" t="s">
+      <c r="B15" s="4" t="s">
         <v>27</v>
       </c>
-      <c r="C15" s="4" t="s">
+      <c r="C15" s="5" t="s">
         <v>29</v>
       </c>
-      <c r="D15" t="s">
+      <c r="D15" s="6" t="s">
         <v>36</v>
       </c>
     </row>
     <row r="16" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="B16" s="5" t="s">
+      <c r="B16" s="4" t="s">
         <v>30</v>
       </c>
-      <c r="C16" s="4" t="s">
+      <c r="C16" s="5" t="s">
         <v>28</v>
       </c>
-      <c r="D16" t="s">
+      <c r="D16" s="6" t="s">
         <v>37</v>
       </c>
     </row>
     <row r="17" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B17" s="5" t="s">
+      <c r="B17" s="4" t="s">
+        <v>56</v>
+      </c>
+      <c r="C17" s="5" t="s">
+        <v>57</v>
+      </c>
+      <c r="D17" s="6" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="18" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B18" s="4" t="s">
         <v>31</v>
       </c>
-      <c r="C17" s="4" t="s">
+      <c r="C18" s="5" t="s">
         <v>32</v>
       </c>
-      <c r="D17" t="s">
+      <c r="D18" s="6" t="s">
         <v>38</v>
       </c>
     </row>
-    <row r="18" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B18" s="5" t="s">
+    <row r="19" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B19" s="4" t="s">
         <v>34</v>
       </c>
-      <c r="C18" s="4" t="s">
+      <c r="C19" s="5" t="s">
         <v>33</v>
       </c>
-      <c r="D18" t="s">
+      <c r="D19" s="6" t="s">
         <v>39</v>
       </c>
     </row>
-    <row r="19" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B19" s="5" t="s">
+    <row r="20" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B20" s="4" t="s">
         <v>40</v>
       </c>
-      <c r="C19" s="4" t="s">
+      <c r="C20" s="5" t="s">
         <v>41</v>
       </c>
-      <c r="D19" t="s">
+      <c r="D20" s="6" t="s">
         <v>42</v>
       </c>
     </row>
-    <row r="20" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B20" s="5" t="s">
+    <row r="21" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B21" s="4" t="s">
         <v>43</v>
       </c>
-      <c r="C20" s="4" t="s">
+      <c r="C21" s="5" t="s">
         <v>55</v>
       </c>
-      <c r="D20" t="s">
+      <c r="D21" s="6" t="s">
         <v>49</v>
       </c>
     </row>
-    <row r="21" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B21" s="5" t="s">
+    <row r="22" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B22" s="4" t="s">
         <v>44</v>
       </c>
-      <c r="D21" t="s">
+      <c r="C22" s="5" t="s">
+        <v>59</v>
+      </c>
+      <c r="D22" s="6" t="s">
         <v>50</v>
       </c>
     </row>
-    <row r="22" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B22" s="5" t="s">
+    <row r="23" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B23" s="4" t="s">
         <v>45</v>
       </c>
-      <c r="D22" t="s">
+      <c r="C23" s="6"/>
+      <c r="D23" s="6" t="s">
         <v>51</v>
       </c>
     </row>
-    <row r="23" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B23" s="5" t="s">
+    <row r="24" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B24" s="4" t="s">
         <v>46</v>
       </c>
-      <c r="D23" t="s">
+      <c r="C24" s="6"/>
+      <c r="D24" s="6" t="s">
         <v>52</v>
       </c>
     </row>
-    <row r="24" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B24" s="5" t="s">
+    <row r="25" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B25" s="4" t="s">
         <v>47</v>
       </c>
-      <c r="D24" t="s">
+      <c r="C25" s="6"/>
+      <c r="D25" s="6" t="s">
         <v>53</v>
       </c>
     </row>
-    <row r="25" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B25" s="5" t="s">
+    <row r="26" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B26" s="4" t="s">
         <v>48</v>
       </c>
-      <c r="D25" t="s">
+      <c r="C26" s="6"/>
+      <c r="D26" s="6" t="s">
         <v>54</v>
-      </c>
-    </row>
-    <row r="29" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="D29" t="s">
-        <v>13</v>
       </c>
     </row>
     <row r="30" spans="2:4" x14ac:dyDescent="0.25">
@@ -790,6 +824,11 @@
     </row>
     <row r="34" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D34" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="35" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D35" t="s">
         <v>13</v>
       </c>
     </row>
@@ -805,11 +844,14 @@
     <hyperlink ref="C14" r:id="rId8"/>
     <hyperlink ref="C15" r:id="rId9"/>
     <hyperlink ref="C16" r:id="rId10"/>
-    <hyperlink ref="C17" r:id="rId11"/>
-    <hyperlink ref="C18" r:id="rId12"/>
-    <hyperlink ref="C19" r:id="rId13"/>
-    <hyperlink ref="C20" r:id="rId14"/>
+    <hyperlink ref="C18" r:id="rId11"/>
+    <hyperlink ref="C19" r:id="rId12"/>
+    <hyperlink ref="C20" r:id="rId13"/>
+    <hyperlink ref="C21" r:id="rId14"/>
+    <hyperlink ref="C17" r:id="rId15"/>
+    <hyperlink ref="C22" r:id="rId16"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId17"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Problem of the day added for Dec 21, 2020
</commit_message>
<xml_diff>
--- a/Practice_Problems_for_Respective_Dates.xlsx
+++ b/Practice_Problems_for_Respective_Dates.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="65" uniqueCount="60">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="66" uniqueCount="61">
   <si>
     <t>Date</t>
   </si>
@@ -204,6 +204,9 @@
   </si>
   <si>
     <t>Minimum and Maximum Element</t>
+  </si>
+  <si>
+    <t>Largest Subarray With 0 Sum</t>
   </si>
 </sst>
 </file>
@@ -566,7 +569,7 @@
   <dimension ref="A6:E35"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A6" workbookViewId="0">
-      <selection activeCell="C22" sqref="C22"/>
+      <selection activeCell="C23" sqref="C23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -770,7 +773,9 @@
       <c r="B23" s="4" t="s">
         <v>45</v>
       </c>
-      <c r="C23" s="6"/>
+      <c r="C23" s="5" t="s">
+        <v>60</v>
+      </c>
       <c r="D23" s="6" t="s">
         <v>51</v>
       </c>
@@ -850,8 +855,9 @@
     <hyperlink ref="C21" r:id="rId14"/>
     <hyperlink ref="C17" r:id="rId15"/>
     <hyperlink ref="C22" r:id="rId16"/>
+    <hyperlink ref="C23" r:id="rId17"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" r:id="rId17"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId18"/>
 </worksheet>
 </file>
</xml_diff>